<commit_message>
Fixed some sonar issues, but mainly fixed the build process to finally produce code coverage also during hte integration test phase.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/commands-failure-test.xlsx
+++ b/conf-core/src/test/resources/dataloader/commands-failure-test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\dataloader-tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-195" yWindow="2145" windowWidth="28620" windowHeight="13170"/>
   </bookViews>
@@ -132,8 +137,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -144,6 +149,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,36 +446,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -475,19 +482,19 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -495,19 +502,19 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="2"/>
@@ -516,16 +523,16 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="2"/>
@@ -534,19 +541,19 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>